<commit_message>
Fix DVI timing constraint error
</commit_message>
<xml_diff>
--- a/Tools/vga_timing.xlsx
+++ b/Tools/vga_timing.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="17">
   <si>
     <t>VGA Timing Calculator</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -467,7 +468,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -661,4 +662,206 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="2" max="3" width="9.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <f>(1/C19)*1000</f>
+        <v>59.333940912888281</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <f>(1/C12)*1000000</f>
+        <v>9137.4269005847946</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <f>25000000/6</f>
+        <v>4166666.6666666665</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1">
+        <v>160</v>
+      </c>
+      <c r="C8">
+        <f>(B8/$B$5)*1000000</f>
+        <v>38.4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1">
+        <v>80</v>
+      </c>
+      <c r="C9">
+        <f t="shared" ref="C9:C12" si="0">(B9/$B$5)*1000000</f>
+        <v>19.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="1">
+        <v>12</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>2.88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="1">
+        <v>204</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>48.96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <f>SUM(B8:B11)</f>
+        <v>456</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>109.44000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="1">
+        <v>144</v>
+      </c>
+      <c r="C15">
+        <f>$C$12/1000*B15</f>
+        <v>15.759360000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <f t="shared" ref="C16:C19" si="1">$C$12/1000*B16</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="1">
+        <v>10</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="1"/>
+        <v>1.0944</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19">
+        <f>SUM(B15:B18)</f>
+        <v>154</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="1"/>
+        <v>16.853760000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Make OAM ram seq write & seq read
</commit_message>
<xml_diff>
--- a/Tools/vga_timing.xlsx
+++ b/Tools/vga_timing.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -468,7 +468,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -493,7 +493,7 @@
       </c>
       <c r="B3">
         <f>(1/C19)*1000</f>
-        <v>59.980806142034545</v>
+        <v>59.297912713472485</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -613,11 +613,11 @@
         <v>6</v>
       </c>
       <c r="B16" s="1">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C16">
         <f t="shared" ref="C16:C19" si="1">$C$12/1000*B16</f>
-        <v>0.28800000000000003</v>
+        <v>0.38400000000000001</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -637,11 +637,11 @@
         <v>8</v>
       </c>
       <c r="B18" s="1">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C18">
         <f t="shared" si="1"/>
-        <v>0.96</v>
+        <v>1.056</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -650,11 +650,11 @@
       </c>
       <c r="B19">
         <f>SUM(B15:B18)</f>
-        <v>521</v>
+        <v>527</v>
       </c>
       <c r="C19">
         <f t="shared" si="1"/>
-        <v>16.672000000000001</v>
+        <v>16.864000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>